<commit_message>
Adding Scenario 5 Test Case 3
</commit_message>
<xml_diff>
--- a/resources/FillupDetailsxlsx.xlsx
+++ b/resources/FillupDetailsxlsx.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\GitHub\IdentifyCourses\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B19246-7404-4B81-8409-E370A16127F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C89572-18A8-4195-84BE-843554A602B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{1F849B88-377B-469A-B917-14E0620FDD96}"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{1F849B88-377B-469A-B917-14E0620FDD96}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstPage" sheetId="1" r:id="rId1"/>
     <sheet name="SecondPage" sheetId="2" r:id="rId2"/>
     <sheet name="ThirdPage" sheetId="3" r:id="rId3"/>
+    <sheet name="FourthPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
   <si>
     <t>Fname</t>
   </si>
@@ -469,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F103F54B-ED0C-4A43-A6F1-96AAE627DAB8}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,4 +746,97 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43412F22-6A32-4FF6-808C-10DE968C2F08}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>9876543210</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A3BD6FFF-7857-4CB0-9A8D-BAAC27CB7F95}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added scenario 5 Test case 7
</commit_message>
<xml_diff>
--- a/resources/FillupDetailsxlsx.xlsx
+++ b/resources/FillupDetailsxlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\GitHub\IdentifyCourses\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E12CBA5-52E9-4747-AEBE-F83CE4D80D1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94CA541-721F-4916-9E18-F545CB52DC8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" activeTab="6" xr2:uid="{1F849B88-377B-469A-B917-14E0620FDD96}"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="7" xr2:uid="{1F849B88-377B-469A-B917-14E0620FDD96}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstPage" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="FifthPage" sheetId="5" r:id="rId5"/>
     <sheet name="SixthPage" sheetId="6" r:id="rId6"/>
     <sheet name="SeventhPage" sheetId="7" r:id="rId7"/>
+    <sheet name="8th Page" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="21">
   <si>
     <t>Fname</t>
   </si>
@@ -48,9 +49,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Instiname</t>
   </si>
   <si>
@@ -94,6 +92,9 @@
   </si>
   <si>
     <t>Orissa</t>
+  </si>
+  <si>
+    <t>Automation</t>
   </si>
 </sst>
 </file>
@@ -471,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F103F54B-ED0C-4A43-A6F1-96AAE627DAB8}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,12 +485,11 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,28 +520,25 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2">
-        <v>9876543210</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -554,9 +551,6 @@
       </c>
       <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -570,10 +564,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D97067A-7917-4FCA-B30C-7FFE9778FA97}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,13 +576,12 @@
     <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -616,25 +609,22 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>9876543210</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -647,9 +637,6 @@
       </c>
       <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -662,10 +649,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFC7916-F6F6-4F55-9BC0-8EA19E1BD588}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,13 +660,12 @@
     <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,25 +693,22 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>9876543210</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -738,9 +721,6 @@
       </c>
       <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -753,10 +733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43412F22-6A32-4FF6-808C-10DE968C2F08}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,14 +745,13 @@
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,25 +779,22 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>9876543210</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -831,9 +807,6 @@
       </c>
       <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -846,15 +819,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95F9B44-A9A4-4031-A503-C5B3F3CF358A}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,25 +855,22 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>9876543210</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -913,9 +883,6 @@
       </c>
       <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -928,19 +895,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B816CDF2-4923-4EE9-82C7-49D065933A69}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,25 +935,22 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
-        <v>9876543210</v>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -999,9 +963,6 @@
       </c>
       <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1013,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9CB044-6CA6-492D-9442-9091EC3D03AB}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,51 +1003,51 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1095,4 +1056,86 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20E472A-1D53-4AB3-87DC-F59FF5235228}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{08A9F5A8-1B93-458B-A4E4-CF15CCD0F2E6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>